<commit_message>
searching in multiple files
</commit_message>
<xml_diff>
--- a/sample_scores2.xlsx
+++ b/sample_scores2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iba\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\python work files\excel searching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82BCA373-6E86-4933-8BA7-AC8F4459A0C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FA1139-5EA7-4641-B765-AD7333EC055F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{A4CB960E-6934-234D-B068-B13526EB200C}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +466,7 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <v>34</v>
@@ -521,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>73</v>
@@ -631,7 +631,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>97</v>

</xml_diff>